<commit_message>
update of participants sheet
</commit_message>
<xml_diff>
--- a/SSXtoolkit_participants.xlsx
+++ b/SSXtoolkit_participants.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="-21600" windowWidth="35940" windowHeight="21140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Workshop 1" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -792,6 +792,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,12 +806,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -845,7 +845,7 @@
         <xdr:cNvPr id="2" name="Imagem 1" descr="BARRA2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1163,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AR31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G8" zoomScale="99" zoomScaleNormal="99" zoomScalePageLayoutView="99" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView tabSelected="1" topLeftCell="N17" zoomScale="99" zoomScaleNormal="99" zoomScalePageLayoutView="99" workbookViewId="0">
+      <selection activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1184,51 +1184,51 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:44" ht="14.5" customHeight="1">
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
     </row>
     <row r="4" spans="1:44" ht="14.5" customHeight="1">
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
     </row>
     <row r="5" spans="1:44" ht="14.5" customHeight="1">
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
     </row>
     <row r="6" spans="1:44" ht="14.5" customHeight="1">
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
     </row>
     <row r="7" spans="1:44" ht="14.5" customHeight="1">
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
     </row>
     <row r="8" spans="1:44" ht="14.5" customHeight="1">
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
     </row>
     <row r="9" spans="1:44" ht="14.5" customHeight="1">
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
     </row>
     <row r="10" spans="1:44" ht="14.5" customHeight="1">
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
     </row>
     <row r="11" spans="1:44" ht="15.5" customHeight="1">
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
     </row>
     <row r="12" spans="1:44" ht="15">
       <c r="G12" s="33"/>
@@ -1238,14 +1238,14 @@
     <row r="13" spans="1:44" ht="15">
       <c r="A13" s="12"/>
       <c r="M13" s="5"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="35"/>
-      <c r="U13" s="35"/>
-      <c r="V13" s="35"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="37"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="37"/>
       <c r="W13" s="17"/>
       <c r="X13" s="18"/>
       <c r="Y13" s="18"/>
@@ -1254,10 +1254,10 @@
       <c r="AB13" s="17"/>
       <c r="AC13" s="19"/>
       <c r="AD13" s="18"/>
-      <c r="AE13" s="35"/>
-      <c r="AF13" s="35"/>
-      <c r="AG13" s="35"/>
-      <c r="AH13" s="35"/>
+      <c r="AE13" s="37"/>
+      <c r="AF13" s="37"/>
+      <c r="AG13" s="37"/>
+      <c r="AH13" s="37"/>
       <c r="AI13" s="18"/>
       <c r="AJ13" s="18"/>
       <c r="AK13" s="4"/>
@@ -1313,16 +1313,16 @@
         <v>9</v>
       </c>
       <c r="O14" s="16"/>
-      <c r="P14" s="37" t="s">
+      <c r="P14" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="Q14" s="38" t="s">
+      <c r="Q14" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="R14" s="38" t="s">
+      <c r="R14" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="S14" s="38" t="s">
+      <c r="S14" s="35" t="s">
         <v>179</v>
       </c>
       <c r="T14" s="20"/>
@@ -1438,6 +1438,18 @@
       <c r="N16" s="15" t="s">
         <v>172</v>
       </c>
+      <c r="P16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>0</v>
+      </c>
+      <c r="R16" s="4">
+        <v>0</v>
+      </c>
+      <c r="S16" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:23" ht="35" customHeight="1">
       <c r="A17" s="13">
@@ -1714,6 +1726,18 @@
       <c r="N22" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:23" ht="35" customHeight="1">
       <c r="A23" s="13">
@@ -1999,6 +2023,18 @@
       <c r="N28" s="1" t="s">
         <v>151</v>
       </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:23" ht="35" customHeight="1">
       <c r="A29" s="13">
@@ -2106,11 +2142,11 @@
     <row r="31" spans="1:23">
       <c r="P31">
         <f>SUM(P15:P30)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q31">
         <f t="shared" ref="Q31:S31" si="0">SUM(Q15:Q30)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R31">
         <f t="shared" si="0"/>
@@ -2118,14 +2154,14 @@
       </c>
       <c r="S31">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U31" t="s">
         <v>180</v>
       </c>
       <c r="W31">
         <f>COUNT(P15:P30)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>